<commit_message>
new contact remark add
</commit_message>
<xml_diff>
--- a/MadhyaPradesh/Guna/Raghogarh, Guna, MP, Schools.xlsx
+++ b/MadhyaPradesh/Guna/Raghogarh, Guna, MP, Schools.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="229">
   <si>
     <t>Find Your School : You Can Find Your School Here.</t>
   </si>
@@ -628,9 +628,6 @@
     <t>7942693534-JD</t>
   </si>
   <si>
-    <t>7697420197 , 9755000536</t>
-  </si>
-  <si>
     <t>9826838717 , 8463888152</t>
   </si>
   <si>
@@ -677,6 +674,33 @@
   </si>
   <si>
     <t>9753797668 , 9893564748 , 7389871365</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>ring</t>
+  </si>
+  <si>
+    <t>invalid number</t>
+  </si>
+  <si>
+    <t>invaild</t>
+  </si>
+  <si>
+    <t>call today evening 8:00 PM</t>
+  </si>
+  <si>
+    <t>State : Madhya PradeshDistrict : GUNABlock : RAGHOGARHVillage : GOVINDPURACluster : HSS Kumbhraj</t>
+  </si>
+  <si>
+    <t>not intrested</t>
+  </si>
+  <si>
+    <t>already software own , but intrested</t>
+  </si>
+  <si>
+    <t>incoming call not available</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B107" workbookViewId="0">
-      <selection activeCell="C122" sqref="C122"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1069,6 +1093,9 @@
       <c r="D2" s="3" t="s">
         <v>202</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
@@ -1105,6 +1132,9 @@
       <c r="D5" s="3">
         <v>9300795532</v>
       </c>
+      <c r="E5" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
@@ -1119,6 +1149,9 @@
       <c r="D6" s="3">
         <v>9893636349</v>
       </c>
+      <c r="E6" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
@@ -1133,6 +1166,9 @@
       <c r="D7" s="3" t="s">
         <v>203</v>
       </c>
+      <c r="E7" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
@@ -1232,11 +1268,14 @@
       <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="3">
+        <v>9755000536</v>
+      </c>
+      <c r="E16" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>23070904103</v>
       </c>
@@ -1247,7 +1286,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>23070904105</v>
       </c>
@@ -1258,7 +1297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>23070904202</v>
       </c>
@@ -1269,7 +1308,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
         <v>23070904403</v>
       </c>
@@ -1280,7 +1319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
         <v>23070904503</v>
       </c>
@@ -1291,7 +1330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
         <v>23070904603</v>
       </c>
@@ -1302,7 +1341,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
         <v>23070904802</v>
       </c>
@@ -1313,10 +1352,13 @@
         <v>36</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>205</v>
+      </c>
+      <c r="E23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
         <v>23070905104</v>
       </c>
@@ -1327,7 +1369,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
         <v>23070905407</v>
       </c>
@@ -1338,7 +1380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
         <v>23070905408</v>
       </c>
@@ -1349,7 +1391,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
         <v>23070905806</v>
       </c>
@@ -1357,13 +1399,16 @@
         <v>44</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>204</v>
+      </c>
+      <c r="E27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
         <v>23070905808</v>
       </c>
@@ -1374,7 +1419,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
         <v>23070906303</v>
       </c>
@@ -1385,7 +1430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" s="2">
         <v>23070906403</v>
       </c>
@@ -1398,8 +1443,11 @@
       <c r="D30" s="3">
         <v>8878447888</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
         <v>23070906408</v>
       </c>
@@ -1410,7 +1458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
         <v>23070906410</v>
       </c>
@@ -1421,10 +1469,13 @@
         <v>48</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>206</v>
+      </c>
+      <c r="E32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>23070906413</v>
       </c>
@@ -1437,8 +1488,11 @@
       <c r="D33" s="3">
         <v>8517917020</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>23070906705</v>
       </c>
@@ -1449,7 +1503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>23070906706</v>
       </c>
@@ -1462,8 +1516,11 @@
       <c r="D35" s="3">
         <v>9589740552</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>23070906804</v>
       </c>
@@ -1476,8 +1533,11 @@
       <c r="D36" s="3">
         <v>9009668848</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>23070906805</v>
       </c>
@@ -1488,7 +1548,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>23070906807</v>
       </c>
@@ -1499,7 +1559,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>23070907911</v>
       </c>
@@ -1510,7 +1570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>23070907913</v>
       </c>
@@ -1521,7 +1581,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>23070907914</v>
       </c>
@@ -1532,7 +1592,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>23070908406</v>
       </c>
@@ -1546,7 +1606,7 @@
         <v>7089277452</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>23070908408</v>
       </c>
@@ -1557,7 +1617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>23070908409</v>
       </c>
@@ -1568,7 +1628,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>23070908410</v>
       </c>
@@ -1582,7 +1642,7 @@
         <v>7089277452</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>23070908603</v>
       </c>
@@ -1593,7 +1653,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <v>23070908604</v>
       </c>
@@ -1604,7 +1664,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" s="2">
         <v>23070908605</v>
       </c>
@@ -1637,7 +1697,7 @@
         <v>75</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1662,7 +1722,7 @@
         <v>75</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1803,7 +1863,7 @@
         <v>86</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1817,7 +1877,7 @@
         <v>86</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1944,7 +2004,7 @@
         <v>86</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2090,7 +2150,7 @@
         <v>121</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2181,7 +2241,7 @@
         <v>136</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2195,7 +2255,7 @@
         <v>136</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2209,7 +2269,7 @@
         <v>139</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2336,7 +2396,7 @@
         <v>161</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2397,7 +2457,7 @@
         <v>169</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2436,7 +2496,7 @@
         <v>173</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2588,7 +2648,7 @@
         <v>197</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="132" spans="1:4">

</xml_diff>